<commit_message>
Updated detailed status spreadsheet
</commit_message>
<xml_diff>
--- a/docs/detailed status.xlsx
+++ b/docs/detailed status.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="160">
   <si>
     <t>Namespace</t>
   </si>
@@ -29,15 +29,9 @@
     <t>Ti.Accelerometer</t>
   </si>
   <si>
-    <t>to do</t>
-  </si>
-  <si>
     <t>Ti.Analytics</t>
   </si>
   <si>
-    <t>To do.</t>
-  </si>
-  <si>
     <t>Ti.API</t>
   </si>
   <si>
@@ -89,9 +83,6 @@
     <t>Ti.Filesystem</t>
   </si>
   <si>
-    <t>Anvil pass. Tests using Buffer and Stream were disabled. Implementation uses HTML5 and works with local storage only.</t>
-  </si>
-  <si>
     <t>Ti.Geolocation</t>
   </si>
   <si>
@@ -122,15 +113,9 @@
     <t>Ti.Media.AudioPlayer</t>
   </si>
   <si>
-    <t>Implemented in full using HTML5 by GL.</t>
-  </si>
-  <si>
     <t>Ti.Media.Sound</t>
   </si>
   <si>
-    <t>Implemented in full using HTML5 by GL.</t>
-  </si>
-  <si>
     <t>Ti.Media.VideoPlayer</t>
   </si>
   <si>
@@ -164,33 +149,21 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Tizen issue prevents from completion. See https://bugs.tizen.org/jira/browse/TDIST-43</t>
-  </si>
-  <si>
     <t>Depends on Ti.Accelerometer, which doesn't work on Tizen.</t>
   </si>
   <si>
     <t>Kitchen sink was fixed to enable operation on Mobile Web. But Tizen implementation requires Tizen facebook client which is not available. See https://developer.tizen.org/forums/web-application-development/facebook-login-tizen</t>
   </si>
   <si>
-    <t>Kitchen sink: fixed, works when GPS is enabled. Web-based geolocation doesn't work; issue is related to Tizen. Mail sent.</t>
-  </si>
-  <si>
     <t>Details</t>
   </si>
   <si>
-    <t>Incomplete MW implementation. GL added functionality using JavaScript (new methods getCurrencyCode, getCurrencySymbol, getLocaleCurrencySymbol, Ti.String.formatCurrency)</t>
-  </si>
-  <si>
     <t>Anvil pass. GL implemented new methods. Everything works, except: clearCookies(host), validateSecureCertificate, tlsVersion, enableKeepAlive, cache.</t>
   </si>
   <si>
     <t>Implemented by GL partially using Tizen Device API. Some functions cannot be implemented due to Tizen API limitations (macaddress, netmask, architecture, availableMemory, processorCount).</t>
   </si>
   <si>
-    <t>Anvil fail; partially works, but has implementation issues related to Tizen. Ti.XML module is based on the "system" component - DOMParser.</t>
-  </si>
-  <si>
     <t>Base UI -&gt; Hide Soft keyboard (Android)</t>
   </si>
   <si>
@@ -287,9 +260,6 @@
     <t>Base UI -&gt; views -&gt; web views-&gt; Basic auth</t>
   </si>
   <si>
-    <t>Tizen's browser doesn't seem to handle HTTP authentication (ignores auth header). Being discussed in Tizen mailing list.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Base UI -&gt; views -&gt; web views-&gt; XHR to FileSystem </t>
   </si>
   <si>
@@ -309,9 +279,6 @@
   </si>
   <si>
     <t>Controls -&gt; Label -&gt; AutoLink</t>
-  </si>
-  <si>
-    <t>This property is Android only. No Tizen equivalent.</t>
   </si>
   <si>
     <t>Controls -&gt; Label -&gt; Basic -&gt; Label 1 Background</t>
@@ -406,10 +373,6 @@
   </si>
   <si>
     <t>Platform -&gt; Application events</t>
-  </si>
-  <si>
-    <t>Such application events are not supported on Tizen.
-In Titanium, only Android 4 platform implements them.</t>
   </si>
   <si>
     <t>Platform -&gt; CommonJs -&gt; test3</t>
@@ -497,9 +460,6 @@
     <t>Base UI -&gt; Window (standalone) -&gt; open (Fullscreen)</t>
   </si>
   <si>
-    <t>Notification area is not covered. Function webkitRequestFullScreen has no effect, although success callback is entered.</t>
-  </si>
-  <si>
     <t>Implemented in HTML5</t>
   </si>
   <si>
@@ -521,10 +481,47 @@
     <t>No Tizen equivalent; webSQL is asynchronous.</t>
   </si>
   <si>
-    <t>CreateAudioPlayer implemented by GL. Some functions implemented in HTML5. The rest of the namespace is not implemented.</t>
-  </si>
-  <si>
     <t>Own test code; Kitchen sink</t>
+  </si>
+  <si>
+    <t>Anvil, own test code</t>
+  </si>
+  <si>
+    <t>Sends and receives responses, but no server stats visible. GL sent request to Appcelerator.</t>
+  </si>
+  <si>
+    <t>Anvil pass. Tests using Buffer and Stream (out of scope) were disabled. Implementation uses HTML5 and works with local storage.</t>
+  </si>
+  <si>
+    <t>Kitchen sink: fixed, works when GPS is enabled. Web-based geolocation doesn't work; issue is related to Tizen (defect opened).</t>
+  </si>
+  <si>
+    <t>Tizen issue prevents from completion. Defect opened.</t>
+  </si>
+  <si>
+    <t>Incomplete MW implementation. GL is adding functionality using JavaScript (new methods getCurrencyCode, getCurrencySymbol, getLocaleCurrencySymbol, Ti.String.formatCurrency); activity currently in progress.</t>
+  </si>
+  <si>
+    <t>Implemented in full using HTML5.</t>
+  </si>
+  <si>
+    <t>Anvil tests are not valid. The core namespace functionality appears to work.</t>
+  </si>
+  <si>
+    <t>Such application events are not supported on Tizen.
+Only Android 4 platform implements them.</t>
+  </si>
+  <si>
+    <t>Ti.UI.Tizen.hideSoftKeyboard() added</t>
+  </si>
+  <si>
+    <t>Tizen's browser doesn't seem to handle HTTP authentication (ignores auth header). Tizen defect opened.</t>
+  </si>
+  <si>
+    <t>Notification area is not covered. Function webkitRequestFullScreen has no effect, although success callback is entered. This appears to be by design.</t>
+  </si>
+  <si>
+    <t>AutoLink property added to Label.</t>
   </si>
 </sst>
 </file>
@@ -917,8 +914,8 @@
         <xdr:to>
           <xdr:col>3</xdr:col>
           <xdr:colOff>371475</xdr:colOff>
-          <xdr:row>1</xdr:row>
-          <xdr:rowOff>304800</xdr:rowOff>
+          <xdr:row>2</xdr:row>
+          <xdr:rowOff>114300</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1239,7 +1236,7 @@
   <dimension ref="A1:T27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1260,7 +1257,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
@@ -1279,287 +1276,287 @@
       <c r="S1" s="9"/>
       <c r="T1" s="9"/>
     </row>
-    <row r="2" spans="1:20" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>49</v>
+        <v>151</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>148</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
         <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
         <v>19</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>149</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>150</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>54</v>
+        <v>152</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B19" s="16" t="s">
-        <v>159</v>
+        <v>34</v>
       </c>
       <c r="C19" s="16" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" t="s">
-        <v>26</v>
+        <v>153</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" t="s">
-        <v>26</v>
+        <v>153</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C24" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>57</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1607,8 +1604,8 @@
               <to>
                 <xdr:col>3</xdr:col>
                 <xdr:colOff>371475</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>304800</xdr:rowOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </to>
             </anchor>
           </objectPr>
@@ -1627,7 +1624,7 @@
   <dimension ref="A1:N221"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1638,18 +1635,18 @@
   <sheetData>
     <row r="1" spans="1:14" ht="65.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
@@ -1665,680 +1662,680 @@
     </row>
     <row r="3" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>62</v>
+        <v>156</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B4" s="17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B5" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:14" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B7" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D7" s="3"/>
     </row>
     <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C8" s="13"/>
       <c r="D8" s="3"/>
     </row>
     <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C9" s="13"/>
       <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C10" s="13"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C12" s="13"/>
       <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:14" s="16" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="D13" s="24"/>
     </row>
     <row r="14" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D15" s="3"/>
     </row>
     <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B16" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="D16" s="3"/>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" ht="39" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B18" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C19" s="18" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C20" s="18"/>
       <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C21" s="18"/>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B22" s="17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C22" s="18" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" ht="39" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B23" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="3"/>
     </row>
     <row r="25" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>90</v>
+        <v>157</v>
       </c>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B26" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C26" s="13"/>
       <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C27" s="18" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B28" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C29" s="18" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B30" s="17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C30" s="18" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>98</v>
+        <v>159</v>
       </c>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="3"/>
     </row>
     <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C33" s="18"/>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="B34" s="20" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C34" s="18" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C35" s="18" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C36" s="18"/>
       <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C37" s="13"/>
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B38" s="25" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C38" s="13"/>
       <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="B39" s="17" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C39" s="18" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D39" s="3"/>
     </row>
     <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="B40" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C40" s="18" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D40" s="3"/>
     </row>
     <row r="41" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C41" s="18" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B42" s="17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C42" s="18" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:4" ht="39" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="B43" s="17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C44" s="18"/>
       <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="19" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C45" s="18" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B46" s="17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C46" s="18" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B47" s="17" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C47" s="18" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="B48" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C48" s="18" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="D48" s="3"/>
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
       <c r="B49" s="17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C49" s="18" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B50" s="17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C50" s="18" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B51" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C51" s="13"/>
       <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="B52" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C52" s="18" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C53" s="18" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
       <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="B54" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C54" s="13"/>
       <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="B55" s="17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C55" s="18" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="D55" s="3"/>
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="19" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="B56" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C56" s="13"/>
       <c r="D56" s="3"/>
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="B57" s="17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C57" s="18" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="19" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="B58" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C58" s="18"/>
       <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C59" s="18" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C60" s="18" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="D60" s="3"/>
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="19" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="B61" s="17" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C61" s="18" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="D61" s="3"/>
     </row>
     <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="B62" s="17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C62" s="13"/>
       <c r="D62" s="3"/>

</xml_diff>